<commit_message>
Cración de pipelines de master_data y pdf
</commit_message>
<xml_diff>
--- a/data/solicitudes/Base_Datos/EmpresaA.xlsx
+++ b/data/solicitudes/Base_Datos/EmpresaA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhuer\OneDrive\Escritorio\COCO\data\solicitudes\Base_Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerardorochabenigno/Documents/ITAM/gran_escala/final/SegurosDelValle/data/solicitudes/Base_Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5809C7-70DE-4CD2-A544-80FE843AE5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBA4604-B2F1-2C48-9B68-4A80AB198125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Nombre</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Nombre15</t>
+  </si>
+  <si>
+    <t>contratante</t>
+  </si>
+  <si>
+    <t>KFC</t>
   </si>
 </sst>
 </file>
@@ -400,143 +406,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B2:B16"/>
+      <selection activeCell="C16" sqref="C2:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>37408</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>37043</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>36678</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>36312</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>35947</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>35582</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>35217</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>34851</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>34486</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1">
         <v>34121</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1">
         <v>33756</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="1">
         <v>33390</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>33025</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1">
         <v>32660</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="1">
         <v>32295</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>